<commit_message>
santa claus 2b y 3a estadistica 3ro bach
</commit_message>
<xml_diff>
--- a/encuestas a padres de familia/estadistica 3ro bachillerato.xlsx
+++ b/encuestas a padres de familia/estadistica 3ro bachillerato.xlsx
@@ -442,8 +442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>